<commit_message>
4 - Botões da home não funcionam 9 - Validar senha do usuário ao editar perfil Bicicleta inserida tem foto default
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha BugFix #1.xlsx
+++ b/Trunk/Doc/Planilha BugFix #1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="7050"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Bug</t>
   </si>
@@ -144,6 +139,12 @@
   </si>
   <si>
     <t>Atenção</t>
+  </si>
+  <si>
+    <t>Botões da Home não funcionam</t>
+  </si>
+  <si>
+    <t>Validar antiga senha do usuário ao editar perfil e trocar senha</t>
   </si>
 </sst>
 </file>
@@ -310,8 +311,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:C16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B1:C16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:C18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B1:C18">
     <filterColumn colId="1">
       <filters>
         <filter val="Douglas Dinarte"/>
@@ -327,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:A16" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:A18" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A18"/>
   <tableColumns count="1">
     <tableColumn id="1" name="#" dataDxfId="0"/>
   </tableColumns>
@@ -337,9 +338,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -377,9 +378,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,7 +415,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,7 +450,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -623,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,6 +821,28 @@
       </c>
       <c r="C16" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizando os bug #03 e #05
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha BugFix #1.xlsx
+++ b/Trunk/Doc/Planilha BugFix #1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="7050"/>
@@ -312,13 +312,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:C18" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B1:C18">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Douglas Dinarte"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:C18"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Bug" dataDxfId="4"/>
     <tableColumn id="2" name="Responsável" dataDxfId="3"/>
@@ -338,9 +332,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -378,7 +372,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -450,7 +444,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -627,7 +621,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -675,21 +669,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -700,18 +694,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -722,7 +716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -733,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -744,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -812,7 +806,7 @@
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
* Ajustei para aparecer o nome da pessoa que te convidou. * Ajustei para que quando entrar num perfil de alguém que já te convidou, já apareçam os botões de Responder e Recusar Convite. * Implementei o StatusRetorno e DescricaoRetorno para tratar possíveis erros retornados do WS. * Ajustei o módulo de bicicletas. Falta apenas ajustar o upload da imagem para o momento de cadastro / alteração.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Planilha BugFix #1.xlsx
+++ b/Trunk/Doc/Planilha BugFix #1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\fusioness\Trunk\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.dinarte\Documents\fusioness\Trunk\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
   <si>
     <t>Bug</t>
   </si>
@@ -165,6 +165,36 @@
   </si>
   <si>
     <t>NOK</t>
+  </si>
+  <si>
+    <t>Na página inicial, além do que está hoje, mostrar os convites pendentes para os eventos.</t>
+  </si>
+  <si>
+    <t>Bruno / Douglas</t>
+  </si>
+  <si>
+    <t>Fazer tratamento para que quando eu convide algum usuário, ao entrar no perfil dele, invés de aparecer pra adicionar de novo, apareça algo do tipo "Aguardando resposta de amizade."</t>
+  </si>
+  <si>
+    <t>No cadastro de bicicleta incluir já a foto ao invés de ter que alterar depois pra poder incluir.</t>
+  </si>
+  <si>
+    <t>No cadastro de evento incluir a foto fazendo UPLOAD ao invés de colocando o link.</t>
+  </si>
+  <si>
+    <t>Fazer tratamento para listas vazias do tipo "Ops, nada foi encontrado aqui."</t>
+  </si>
+  <si>
+    <t>Fazer o tratamento para Rotas Cadastradas e Rotas Realizadas e mudar a exibição das rotas para que ao invés da LISTA, fique uns mapinhas (se possível).</t>
+  </si>
+  <si>
+    <t>Fazer a validação dos campos da tela de eventos.</t>
+  </si>
+  <si>
+    <t>Criar listagem na tela de eventos para "Eventos que vou participar" e retornar os eventos para os quais você se inscreveu.</t>
+  </si>
+  <si>
+    <t>Na opção EXPLORE está trazendo eventos que são meus (criados). Nâo deve trazer. Verificar se de repente não é melhor deixar apenas a lista de eventos EXPLORE e uma outra que busque por nome, do que deixar o menu LISTA DE EVENTOS, pois são bastante similares.</t>
   </si>
 </sst>
 </file>
@@ -228,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -258,11 +288,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -287,27 +345,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.249977111117893"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -322,30 +359,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:C21" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:C21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="B1:C21"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Bug" dataDxfId="1"/>
-    <tableColumn id="2" name="Responsável" dataDxfId="0"/>
+    <tableColumn id="1" name="Bug" dataDxfId="4"/>
+    <tableColumn id="2" name="Responsável" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:A21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:A30" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:A30"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="#" dataDxfId="4"/>
+    <tableColumn id="1" name="#" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -383,7 +420,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -455,7 +492,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -629,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,30 +939,30 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -942,6 +979,135 @@
       <c r="D21" s="9" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>27</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>28</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>29</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>